<commit_message>
add new command(doc for send .xlsx file from STRH) and fix bug for delete rebuke
</commit_message>
<xml_diff>
--- a/rebuke.xlsx
+++ b/rebuke.xlsx
@@ -490,13 +490,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
         <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>

</xml_diff>